<commit_message>
Updated Commit with File rename functionality v1.0
</commit_message>
<xml_diff>
--- a/Affirm/src/main/java/Affirm_Sheet.xlsx
+++ b/Affirm/src/main/java/Affirm_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Execution_Plan" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="145">
   <si>
     <t>TC_Name</t>
   </si>
@@ -370,6 +370,99 @@
   </si>
   <si>
     <t>%Vandematram2019</t>
+  </si>
+  <si>
+    <t>LPLC009PDB</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Individually Owned</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Non-Qualified</t>
+  </si>
+  <si>
+    <t>Alachua</t>
+  </si>
+  <si>
+    <t>IEBSHR21</t>
+  </si>
+  <si>
+    <t>Add Check</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>112989</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>NQ,Bene</t>
+  </si>
+  <si>
+    <t>Test,Lname</t>
+  </si>
+  <si>
+    <t>Owner,Bene</t>
+  </si>
+  <si>
+    <t>Annuitant,</t>
+  </si>
+  <si>
+    <t>Male,Male</t>
+  </si>
+  <si>
+    <t>10101956,'01011960</t>
+  </si>
+  <si>
+    <t>123456789,'098765432</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>20 Drury Cres</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Return of Premium Death Benefit</t>
+  </si>
+  <si>
+    <t>NASDAQ 100 1 Year -10% Buffer,MSCI EM 1 Year -10% Buffer</t>
+  </si>
+  <si>
+    <t>Funds Percentage</t>
+  </si>
+  <si>
+    <t>50,'50</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>AXA92839</t>
   </si>
 </sst>
 </file>
@@ -755,7 +848,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,7 +918,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -837,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +1009,33 @@
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1065,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,6 +1221,21 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1142,7 +1277,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,6 +1316,24 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1221,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,6 +1507,15 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1395,7 +1557,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1609,21 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1495,7 +1671,7 @@
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,6 +1818,51 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1683,7 +1904,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,6 +1941,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1761,7 +1985,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,19 +2050,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1851,38 +2076,47 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>

</xml_diff>